<commit_message>
Pendiente parametrizar metodo excel
</commit_message>
<xml_diff>
--- a/tareas/src/main/resources/static/doc/Registro.xlsx
+++ b/tareas/src/main/resources/static/doc/Registro.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
   <si>
     <t xml:space="preserve">Código</t>
   </si>
@@ -215,7 +215,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
@@ -440,6 +440,62 @@
         <v>41.0</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" t="n">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" t="n">
+        <v>41.0</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
añadido menu hover para las opciones del registro.
</commit_message>
<xml_diff>
--- a/tareas/src/main/resources/static/doc/Registro.xlsx
+++ b/tareas/src/main/resources/static/doc/Registro.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="99">
   <si>
     <t>Código</t>
   </si>
@@ -149,6 +149,174 @@
   </si>
   <si>
     <t>Sun Sep 20 00:50:47 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 00:50:38 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 00:53:07 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 00:53:08 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 00:53:09 CEST 2020</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 00:53:12 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 00:53:17 CEST 2020</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 00:53:10 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 00:53:22 CEST 2020</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 10:36:23 CEST 2020</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 10:36:25 CEST 2020</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 10:36:26 CEST 2020</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 10:38:10 CEST 2020</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 10:38:19 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 10:44:11 CEST 2020</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 10:44:13 CEST 2020</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 10:44:19 CEST 2020</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 10:44:26 CEST 2020</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 10:44:38 CEST 2020</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 10:45:23 CEST 2020</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 10:45:26 CEST 2020</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 10:44:39 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 10:46:30 CEST 2020</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 10:47:08 CEST 2020</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 10:47:14 CEST 2020</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 10:47:20 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 15:47:26 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 15:47:42 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 15:47:28 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 15:47:50 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 15:47:35 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 15:48:14 CEST 2020</t>
+  </si>
+  <si>
+    <t>The Passionate Programmer</t>
+  </si>
+  <si>
+    <t>Chad Fowler</t>
+  </si>
+  <si>
+    <t>Software Craftmanship</t>
+  </si>
+  <si>
+    <t>Pete McBreen</t>
+  </si>
+  <si>
+    <t>The Art of Agile Development</t>
+  </si>
+  <si>
+    <t>James Shore</t>
+  </si>
+  <si>
+    <t>Continuous Delivery</t>
+  </si>
+  <si>
+    <t>Jez Humble</t>
   </si>
 </sst>
 </file>
@@ -507,7 +675,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -836,6 +1004,1290 @@
         <v>22</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>20.0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23.0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" t="s">
+        <v>52</v>
+      </c>
+      <c r="F24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" t="s">
+        <v>54</v>
+      </c>
+      <c r="F25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26.0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" t="s">
+        <v>58</v>
+      </c>
+      <c r="F27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27.0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" t="s">
+        <v>60</v>
+      </c>
+      <c r="F28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" t="s">
+        <v>56</v>
+      </c>
+      <c r="E29" t="s">
+        <v>62</v>
+      </c>
+      <c r="F29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" t="s">
+        <v>60</v>
+      </c>
+      <c r="E30" t="s">
+        <v>63</v>
+      </c>
+      <c r="F30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>30.0</v>
+      </c>
+      <c r="B31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" t="s">
+        <v>62</v>
+      </c>
+      <c r="E31" t="s">
+        <v>65</v>
+      </c>
+      <c r="F31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" t="s">
+        <v>67</v>
+      </c>
+      <c r="F32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>32.0</v>
+      </c>
+      <c r="B33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" t="s">
+        <v>19</v>
+      </c>
+      <c r="D33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E33" t="s">
+        <v>69</v>
+      </c>
+      <c r="F33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="B34" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" t="s">
+        <v>58</v>
+      </c>
+      <c r="E34" t="s">
+        <v>71</v>
+      </c>
+      <c r="F34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>34.0</v>
+      </c>
+      <c r="B35" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" t="s">
+        <v>18</v>
+      </c>
+      <c r="D35" t="s">
+        <v>67</v>
+      </c>
+      <c r="E35" t="s">
+        <v>73</v>
+      </c>
+      <c r="F35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="B36" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" t="s">
+        <v>69</v>
+      </c>
+      <c r="E36" t="s">
+        <v>75</v>
+      </c>
+      <c r="F36" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>36.0</v>
+      </c>
+      <c r="B37" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" t="s">
+        <v>77</v>
+      </c>
+      <c r="E37" t="s">
+        <v>78</v>
+      </c>
+      <c r="F37" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>37.0</v>
+      </c>
+      <c r="B38" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" t="s">
+        <v>73</v>
+      </c>
+      <c r="E38" t="s">
+        <v>80</v>
+      </c>
+      <c r="F38" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="B39" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39" t="s">
+        <v>78</v>
+      </c>
+      <c r="E39" t="s">
+        <v>82</v>
+      </c>
+      <c r="F39" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>39.0</v>
+      </c>
+      <c r="B40" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" t="s">
+        <v>75</v>
+      </c>
+      <c r="E40" t="s">
+        <v>84</v>
+      </c>
+      <c r="F40" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="B41" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" t="s">
+        <v>85</v>
+      </c>
+      <c r="E41" t="s">
+        <v>86</v>
+      </c>
+      <c r="F41" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>41.0</v>
+      </c>
+      <c r="B42" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" t="s">
+        <v>87</v>
+      </c>
+      <c r="E42" t="s">
+        <v>88</v>
+      </c>
+      <c r="F42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>42.0</v>
+      </c>
+      <c r="B43" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" t="s">
+        <v>19</v>
+      </c>
+      <c r="D43" t="s">
+        <v>89</v>
+      </c>
+      <c r="E43" t="s">
+        <v>90</v>
+      </c>
+      <c r="F43" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>43.0</v>
+      </c>
+      <c r="B44" t="s">
+        <v>91</v>
+      </c>
+      <c r="C44" t="s">
+        <v>92</v>
+      </c>
+      <c r="D44" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="B45" t="s">
+        <v>93</v>
+      </c>
+      <c r="C45" t="s">
+        <v>94</v>
+      </c>
+      <c r="D45" t="n">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="B46" t="s">
+        <v>95</v>
+      </c>
+      <c r="C46" t="s">
+        <v>96</v>
+      </c>
+      <c r="D46" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46.0</v>
+      </c>
+      <c r="B47" t="s">
+        <v>97</v>
+      </c>
+      <c r="C47" t="s">
+        <v>98</v>
+      </c>
+      <c r="D47" t="n">
+        <v>41.0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47.0</v>
+      </c>
+      <c r="B48" t="s">
+        <v>91</v>
+      </c>
+      <c r="C48" t="s">
+        <v>92</v>
+      </c>
+      <c r="D48" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48.0</v>
+      </c>
+      <c r="B49" t="s">
+        <v>93</v>
+      </c>
+      <c r="C49" t="s">
+        <v>94</v>
+      </c>
+      <c r="D49" t="n">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49.0</v>
+      </c>
+      <c r="B50" t="s">
+        <v>95</v>
+      </c>
+      <c r="C50" t="s">
+        <v>96</v>
+      </c>
+      <c r="D50" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50.0</v>
+      </c>
+      <c r="B51" t="s">
+        <v>97</v>
+      </c>
+      <c r="C51" t="s">
+        <v>98</v>
+      </c>
+      <c r="D51" t="n">
+        <v>41.0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>51.0</v>
+      </c>
+      <c r="B52" t="s">
+        <v>91</v>
+      </c>
+      <c r="C52" t="s">
+        <v>92</v>
+      </c>
+      <c r="D52" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>52.0</v>
+      </c>
+      <c r="B53" t="s">
+        <v>93</v>
+      </c>
+      <c r="C53" t="s">
+        <v>94</v>
+      </c>
+      <c r="D53" t="n">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>53.0</v>
+      </c>
+      <c r="B54" t="s">
+        <v>95</v>
+      </c>
+      <c r="C54" t="s">
+        <v>96</v>
+      </c>
+      <c r="D54" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>54.0</v>
+      </c>
+      <c r="B55" t="s">
+        <v>97</v>
+      </c>
+      <c r="C55" t="s">
+        <v>98</v>
+      </c>
+      <c r="D55" t="n">
+        <v>41.0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>55.0</v>
+      </c>
+      <c r="B56" t="s">
+        <v>91</v>
+      </c>
+      <c r="C56" t="s">
+        <v>92</v>
+      </c>
+      <c r="D56" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>56.0</v>
+      </c>
+      <c r="B57" t="s">
+        <v>93</v>
+      </c>
+      <c r="C57" t="s">
+        <v>94</v>
+      </c>
+      <c r="D57" t="n">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>57.0</v>
+      </c>
+      <c r="B58" t="s">
+        <v>95</v>
+      </c>
+      <c r="C58" t="s">
+        <v>96</v>
+      </c>
+      <c r="D58" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>58.0</v>
+      </c>
+      <c r="B59" t="s">
+        <v>97</v>
+      </c>
+      <c r="C59" t="s">
+        <v>98</v>
+      </c>
+      <c r="D59" t="n">
+        <v>41.0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>59.0</v>
+      </c>
+      <c r="B60" t="s">
+        <v>91</v>
+      </c>
+      <c r="C60" t="s">
+        <v>92</v>
+      </c>
+      <c r="D60" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>60.0</v>
+      </c>
+      <c r="B61" t="s">
+        <v>93</v>
+      </c>
+      <c r="C61" t="s">
+        <v>94</v>
+      </c>
+      <c r="D61" t="n">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>61.0</v>
+      </c>
+      <c r="B62" t="s">
+        <v>95</v>
+      </c>
+      <c r="C62" t="s">
+        <v>96</v>
+      </c>
+      <c r="D62" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>62.0</v>
+      </c>
+      <c r="B63" t="s">
+        <v>97</v>
+      </c>
+      <c r="C63" t="s">
+        <v>98</v>
+      </c>
+      <c r="D63" t="n">
+        <v>41.0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>63.0</v>
+      </c>
+      <c r="B64" t="s">
+        <v>91</v>
+      </c>
+      <c r="C64" t="s">
+        <v>92</v>
+      </c>
+      <c r="D64" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>64.0</v>
+      </c>
+      <c r="B65" t="s">
+        <v>93</v>
+      </c>
+      <c r="C65" t="s">
+        <v>94</v>
+      </c>
+      <c r="D65" t="n">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>65.0</v>
+      </c>
+      <c r="B66" t="s">
+        <v>95</v>
+      </c>
+      <c r="C66" t="s">
+        <v>96</v>
+      </c>
+      <c r="D66" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="B67" t="s">
+        <v>97</v>
+      </c>
+      <c r="C67" t="s">
+        <v>98</v>
+      </c>
+      <c r="D67" t="n">
+        <v>41.0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>67.0</v>
+      </c>
+      <c r="B68" t="s">
+        <v>91</v>
+      </c>
+      <c r="C68" t="s">
+        <v>92</v>
+      </c>
+      <c r="D68" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>68.0</v>
+      </c>
+      <c r="B69" t="s">
+        <v>93</v>
+      </c>
+      <c r="C69" t="s">
+        <v>94</v>
+      </c>
+      <c r="D69" t="n">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>69.0</v>
+      </c>
+      <c r="B70" t="s">
+        <v>95</v>
+      </c>
+      <c r="C70" t="s">
+        <v>96</v>
+      </c>
+      <c r="D70" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>70.0</v>
+      </c>
+      <c r="B71" t="s">
+        <v>97</v>
+      </c>
+      <c r="C71" t="s">
+        <v>98</v>
+      </c>
+      <c r="D71" t="n">
+        <v>41.0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>71.0</v>
+      </c>
+      <c r="B72" t="s">
+        <v>91</v>
+      </c>
+      <c r="C72" t="s">
+        <v>92</v>
+      </c>
+      <c r="D72" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>72.0</v>
+      </c>
+      <c r="B73" t="s">
+        <v>93</v>
+      </c>
+      <c r="C73" t="s">
+        <v>94</v>
+      </c>
+      <c r="D73" t="n">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>73.0</v>
+      </c>
+      <c r="B74" t="s">
+        <v>95</v>
+      </c>
+      <c r="C74" t="s">
+        <v>96</v>
+      </c>
+      <c r="D74" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>74.0</v>
+      </c>
+      <c r="B75" t="s">
+        <v>97</v>
+      </c>
+      <c r="C75" t="s">
+        <v>98</v>
+      </c>
+      <c r="D75" t="n">
+        <v>41.0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>75.0</v>
+      </c>
+      <c r="B76" t="s">
+        <v>91</v>
+      </c>
+      <c r="C76" t="s">
+        <v>92</v>
+      </c>
+      <c r="D76" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>76.0</v>
+      </c>
+      <c r="B77" t="s">
+        <v>93</v>
+      </c>
+      <c r="C77" t="s">
+        <v>94</v>
+      </c>
+      <c r="D77" t="n">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>77.0</v>
+      </c>
+      <c r="B78" t="s">
+        <v>95</v>
+      </c>
+      <c r="C78" t="s">
+        <v>96</v>
+      </c>
+      <c r="D78" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>78.0</v>
+      </c>
+      <c r="B79" t="s">
+        <v>97</v>
+      </c>
+      <c r="C79" t="s">
+        <v>98</v>
+      </c>
+      <c r="D79" t="n">
+        <v>41.0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>79.0</v>
+      </c>
+      <c r="B80" t="s">
+        <v>91</v>
+      </c>
+      <c r="C80" t="s">
+        <v>92</v>
+      </c>
+      <c r="D80" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>80.0</v>
+      </c>
+      <c r="B81" t="s">
+        <v>93</v>
+      </c>
+      <c r="C81" t="s">
+        <v>94</v>
+      </c>
+      <c r="D81" t="n">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>81.0</v>
+      </c>
+      <c r="B82" t="s">
+        <v>95</v>
+      </c>
+      <c r="C82" t="s">
+        <v>96</v>
+      </c>
+      <c r="D82" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>82.0</v>
+      </c>
+      <c r="B83" t="s">
+        <v>97</v>
+      </c>
+      <c r="C83" t="s">
+        <v>98</v>
+      </c>
+      <c r="D83" t="n">
+        <v>41.0</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>83.0</v>
+      </c>
+      <c r="B84" t="s">
+        <v>91</v>
+      </c>
+      <c r="C84" t="s">
+        <v>92</v>
+      </c>
+      <c r="D84" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>84.0</v>
+      </c>
+      <c r="B85" t="s">
+        <v>93</v>
+      </c>
+      <c r="C85" t="s">
+        <v>94</v>
+      </c>
+      <c r="D85" t="n">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>85.0</v>
+      </c>
+      <c r="B86" t="s">
+        <v>95</v>
+      </c>
+      <c r="C86" t="s">
+        <v>96</v>
+      </c>
+      <c r="D86" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>86.0</v>
+      </c>
+      <c r="B87" t="s">
+        <v>97</v>
+      </c>
+      <c r="C87" t="s">
+        <v>98</v>
+      </c>
+      <c r="D87" t="n">
+        <v>41.0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>87.0</v>
+      </c>
+      <c r="B88" t="s">
+        <v>91</v>
+      </c>
+      <c r="C88" t="s">
+        <v>92</v>
+      </c>
+      <c r="D88" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>88.0</v>
+      </c>
+      <c r="B89" t="s">
+        <v>93</v>
+      </c>
+      <c r="C89" t="s">
+        <v>94</v>
+      </c>
+      <c r="D89" t="n">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>89.0</v>
+      </c>
+      <c r="B90" t="s">
+        <v>95</v>
+      </c>
+      <c r="C90" t="s">
+        <v>96</v>
+      </c>
+      <c r="D90" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>90.0</v>
+      </c>
+      <c r="B91" t="s">
+        <v>97</v>
+      </c>
+      <c r="C91" t="s">
+        <v>98</v>
+      </c>
+      <c r="D91" t="n">
+        <v>41.0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>91.0</v>
+      </c>
+      <c r="B92" t="s">
+        <v>91</v>
+      </c>
+      <c r="C92" t="s">
+        <v>92</v>
+      </c>
+      <c r="D92" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>92.0</v>
+      </c>
+      <c r="B93" t="s">
+        <v>93</v>
+      </c>
+      <c r="C93" t="s">
+        <v>94</v>
+      </c>
+      <c r="D93" t="n">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>93.0</v>
+      </c>
+      <c r="B94" t="s">
+        <v>95</v>
+      </c>
+      <c r="C94" t="s">
+        <v>96</v>
+      </c>
+      <c r="D94" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>94.0</v>
+      </c>
+      <c r="B95" t="s">
+        <v>97</v>
+      </c>
+      <c r="C95" t="s">
+        <v>98</v>
+      </c>
+      <c r="D95" t="n">
+        <v>41.0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>95.0</v>
+      </c>
+      <c r="B96" t="s">
+        <v>91</v>
+      </c>
+      <c r="C96" t="s">
+        <v>92</v>
+      </c>
+      <c r="D96" t="n">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>96.0</v>
+      </c>
+      <c r="B97" t="s">
+        <v>93</v>
+      </c>
+      <c r="C97" t="s">
+        <v>94</v>
+      </c>
+      <c r="D97" t="n">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>97.0</v>
+      </c>
+      <c r="B98" t="s">
+        <v>95</v>
+      </c>
+      <c r="C98" t="s">
+        <v>96</v>
+      </c>
+      <c r="D98" t="n">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>98.0</v>
+      </c>
+      <c r="B99" t="s">
+        <v>97</v>
+      </c>
+      <c r="C99" t="s">
+        <v>98</v>
+      </c>
+      <c r="D99" t="n">
+        <v>41.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modificaciones en el registro del excel
</commit_message>
<xml_diff>
--- a/tareas/src/main/resources/static/doc/Registro.xlsx
+++ b/tareas/src/main/resources/static/doc/Registro.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="136">
   <si>
     <t>Código</t>
   </si>
@@ -317,6 +317,117 @@
   </si>
   <si>
     <t>Jez Humble</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 23:35:17 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 23:35:19 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 23:35:25 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 23:33:19 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 23:35:34 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 23:31:44 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 23:35:40 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 23:37:31 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 23:37:33 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 23:37:34 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 23:37:40 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 23:37:44 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 23:37:50 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 23:39:05 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 23:37:45 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 23:40:47 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 23:41:11 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 23:42:24 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 23:42:30 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 23:42:38 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 23:42:56 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 23:43:09 CEST 2020</t>
+  </si>
+  <si>
+    <t>Sun Sep 20 23:43:18 CEST 2020</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Mon Sep 21 00:06:26 CEST 2020</t>
+  </si>
+  <si>
+    <t>Mon Sep 21 00:06:31 CEST 2020</t>
+  </si>
+  <si>
+    <t>Mon Sep 21 00:24:59 CEST 2020</t>
+  </si>
+  <si>
+    <t>kk</t>
+  </si>
+  <si>
+    <t>Mon Sep 21 00:25:30 CEST 2020</t>
+  </si>
+  <si>
+    <t>Mon Sep 21 00:26:48 CEST 2020</t>
+  </si>
+  <si>
+    <t>kike</t>
+  </si>
+  <si>
+    <t>Mon Sep 21 00:33:17 CEST 2020</t>
+  </si>
+  <si>
+    <t>Mon Sep 21 00:33:24 CEST 2020</t>
+  </si>
+  <si>
+    <t>programacion</t>
+  </si>
+  <si>
+    <t>Mon Sep 21 00:36:42 CEST 2020</t>
+  </si>
+  <si>
+    <t>Mon Sep 21 00:36:49 CEST 2020</t>
+  </si>
+  <si>
+    <t>asdfa</t>
   </si>
 </sst>
 </file>
@@ -675,7 +786,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F99"/>
+  <dimension ref="A1:F125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2288,6 +2399,526 @@
         <v>41.0</v>
       </c>
     </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>99.0</v>
+      </c>
+      <c r="B100" t="s">
+        <v>18</v>
+      </c>
+      <c r="C100" t="s">
+        <v>19</v>
+      </c>
+      <c r="D100" t="s">
+        <v>99</v>
+      </c>
+      <c r="E100" t="s">
+        <v>100</v>
+      </c>
+      <c r="F100" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="B101" t="s">
+        <v>34</v>
+      </c>
+      <c r="C101" t="s">
+        <v>19</v>
+      </c>
+      <c r="D101" t="s">
+        <v>100</v>
+      </c>
+      <c r="E101" t="s">
+        <v>101</v>
+      </c>
+      <c r="F101" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>101.0</v>
+      </c>
+      <c r="B102" t="s">
+        <v>19</v>
+      </c>
+      <c r="C102" t="s">
+        <v>18</v>
+      </c>
+      <c r="D102" t="s">
+        <v>102</v>
+      </c>
+      <c r="E102" t="s">
+        <v>103</v>
+      </c>
+      <c r="F102" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>102.0</v>
+      </c>
+      <c r="B103" t="s">
+        <v>23</v>
+      </c>
+      <c r="C103" t="s">
+        <v>23</v>
+      </c>
+      <c r="D103" t="s">
+        <v>104</v>
+      </c>
+      <c r="E103" t="s">
+        <v>105</v>
+      </c>
+      <c r="F103" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>103.0</v>
+      </c>
+      <c r="B104" t="s">
+        <v>26</v>
+      </c>
+      <c r="C104" t="s">
+        <v>19</v>
+      </c>
+      <c r="D104" t="s">
+        <v>101</v>
+      </c>
+      <c r="E104" t="s">
+        <v>106</v>
+      </c>
+      <c r="F104" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>104.0</v>
+      </c>
+      <c r="B105" t="s">
+        <v>47</v>
+      </c>
+      <c r="C105" t="s">
+        <v>18</v>
+      </c>
+      <c r="D105" t="s">
+        <v>103</v>
+      </c>
+      <c r="E105" t="s">
+        <v>107</v>
+      </c>
+      <c r="F105" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>105.0</v>
+      </c>
+      <c r="B106" t="s">
+        <v>30</v>
+      </c>
+      <c r="C106" t="s">
+        <v>23</v>
+      </c>
+      <c r="D106" t="s">
+        <v>105</v>
+      </c>
+      <c r="E106" t="s">
+        <v>108</v>
+      </c>
+      <c r="F106" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>106.0</v>
+      </c>
+      <c r="B107" t="s">
+        <v>55</v>
+      </c>
+      <c r="C107" t="s">
+        <v>23</v>
+      </c>
+      <c r="D107" t="s">
+        <v>108</v>
+      </c>
+      <c r="E107" t="s">
+        <v>109</v>
+      </c>
+      <c r="F107" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>107.0</v>
+      </c>
+      <c r="B108" t="s">
+        <v>53</v>
+      </c>
+      <c r="C108" t="s">
+        <v>18</v>
+      </c>
+      <c r="D108" t="s">
+        <v>107</v>
+      </c>
+      <c r="E108" t="s">
+        <v>110</v>
+      </c>
+      <c r="F108" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>108.0</v>
+      </c>
+      <c r="B109" t="s">
+        <v>50</v>
+      </c>
+      <c r="C109" t="s">
+        <v>19</v>
+      </c>
+      <c r="D109" t="s">
+        <v>106</v>
+      </c>
+      <c r="E109" t="s">
+        <v>111</v>
+      </c>
+      <c r="F109" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>109.0</v>
+      </c>
+      <c r="B110" t="s">
+        <v>57</v>
+      </c>
+      <c r="C110" t="s">
+        <v>23</v>
+      </c>
+      <c r="D110" t="s">
+        <v>109</v>
+      </c>
+      <c r="E110" t="s">
+        <v>112</v>
+      </c>
+      <c r="F110" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>110.0</v>
+      </c>
+      <c r="B111" t="s">
+        <v>59</v>
+      </c>
+      <c r="C111" t="s">
+        <v>18</v>
+      </c>
+      <c r="D111" t="s">
+        <v>113</v>
+      </c>
+      <c r="E111" t="s">
+        <v>114</v>
+      </c>
+      <c r="F111" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>111.0</v>
+      </c>
+      <c r="B112" t="s">
+        <v>61</v>
+      </c>
+      <c r="C112" t="s">
+        <v>19</v>
+      </c>
+      <c r="D112" t="s">
+        <v>111</v>
+      </c>
+      <c r="E112" t="s">
+        <v>115</v>
+      </c>
+      <c r="F112" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>112.0</v>
+      </c>
+      <c r="B113" t="s">
+        <v>70</v>
+      </c>
+      <c r="C113" t="s">
+        <v>23</v>
+      </c>
+      <c r="D113" t="s">
+        <v>112</v>
+      </c>
+      <c r="E113" t="s">
+        <v>116</v>
+      </c>
+      <c r="F113" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>113.0</v>
+      </c>
+      <c r="B114" t="s">
+        <v>15</v>
+      </c>
+      <c r="C114" t="s">
+        <v>18</v>
+      </c>
+      <c r="D114" t="s">
+        <v>114</v>
+      </c>
+      <c r="E114" t="s">
+        <v>117</v>
+      </c>
+      <c r="F114" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>114.0</v>
+      </c>
+      <c r="B115" t="s">
+        <v>64</v>
+      </c>
+      <c r="C115" t="s">
+        <v>19</v>
+      </c>
+      <c r="D115" t="s">
+        <v>115</v>
+      </c>
+      <c r="E115" t="s">
+        <v>118</v>
+      </c>
+      <c r="F115" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>115.0</v>
+      </c>
+      <c r="B116" t="s">
+        <v>68</v>
+      </c>
+      <c r="C116" t="s">
+        <v>23</v>
+      </c>
+      <c r="D116" t="s">
+        <v>116</v>
+      </c>
+      <c r="E116" t="s">
+        <v>119</v>
+      </c>
+      <c r="F116" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>116.0</v>
+      </c>
+      <c r="B117" t="s">
+        <v>66</v>
+      </c>
+      <c r="C117" t="s">
+        <v>18</v>
+      </c>
+      <c r="D117" t="s">
+        <v>117</v>
+      </c>
+      <c r="E117" t="s">
+        <v>120</v>
+      </c>
+      <c r="F117" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>117.0</v>
+      </c>
+      <c r="B118" t="s">
+        <v>72</v>
+      </c>
+      <c r="C118" t="s">
+        <v>19</v>
+      </c>
+      <c r="D118" t="s">
+        <v>118</v>
+      </c>
+      <c r="E118" t="s">
+        <v>121</v>
+      </c>
+      <c r="F118" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>118.0</v>
+      </c>
+      <c r="B119" t="s">
+        <v>23</v>
+      </c>
+      <c r="C119" t="s">
+        <v>122</v>
+      </c>
+      <c r="D119" t="s">
+        <v>22</v>
+      </c>
+      <c r="E119" t="s">
+        <v>123</v>
+      </c>
+      <c r="F119" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>119.0</v>
+      </c>
+      <c r="B120" t="s">
+        <v>18</v>
+      </c>
+      <c r="C120" t="s">
+        <v>122</v>
+      </c>
+      <c r="D120" t="s">
+        <v>22</v>
+      </c>
+      <c r="E120" t="s">
+        <v>124</v>
+      </c>
+      <c r="F120" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>120.0</v>
+      </c>
+      <c r="B121" t="s">
+        <v>34</v>
+      </c>
+      <c r="C121" t="s">
+        <v>122</v>
+      </c>
+      <c r="D121" t="s">
+        <v>22</v>
+      </c>
+      <c r="E121" t="s">
+        <v>125</v>
+      </c>
+      <c r="F121" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>121.0</v>
+      </c>
+      <c r="B122" t="s">
+        <v>26</v>
+      </c>
+      <c r="C122" t="s">
+        <v>122</v>
+      </c>
+      <c r="D122" t="s">
+        <v>22</v>
+      </c>
+      <c r="E122" t="s">
+        <v>127</v>
+      </c>
+      <c r="F122" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>122.0</v>
+      </c>
+      <c r="B123" t="s">
+        <v>47</v>
+      </c>
+      <c r="C123" t="s">
+        <v>122</v>
+      </c>
+      <c r="D123" t="s">
+        <v>22</v>
+      </c>
+      <c r="E123" t="s">
+        <v>128</v>
+      </c>
+      <c r="F123" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>123.0</v>
+      </c>
+      <c r="B124" t="s">
+        <v>18</v>
+      </c>
+      <c r="C124" t="s">
+        <v>18</v>
+      </c>
+      <c r="D124" t="s">
+        <v>130</v>
+      </c>
+      <c r="E124" t="s">
+        <v>131</v>
+      </c>
+      <c r="F124" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>124.0</v>
+      </c>
+      <c r="B125" t="s">
+        <v>34</v>
+      </c>
+      <c r="C125" t="s">
+        <v>34</v>
+      </c>
+      <c r="D125" t="s">
+        <v>133</v>
+      </c>
+      <c r="E125" t="s">
+        <v>134</v>
+      </c>
+      <c r="F125" t="s">
+        <v>135</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Menú hover y ventanas modales en el listado de activos
</commit_message>
<xml_diff>
--- a/tareas/src/main/resources/static/doc/Registro.xlsx
+++ b/tareas/src/main/resources/static/doc/Registro.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="148">
   <si>
     <t>Código</t>
   </si>
@@ -428,6 +428,42 @@
   </si>
   <si>
     <t>asdfa</t>
+  </si>
+  <si>
+    <t>Tue Sep 22 22:28:06 CEST 2020</t>
+  </si>
+  <si>
+    <t>Tue Sep 22 22:53:52 CEST 2020</t>
+  </si>
+  <si>
+    <t>activo 1</t>
+  </si>
+  <si>
+    <t>Tue Sep 22 22:54:14 CEST 2020</t>
+  </si>
+  <si>
+    <t>Tue Sep 22 22:54:38 CEST 2020</t>
+  </si>
+  <si>
+    <t>de espera activo 2</t>
+  </si>
+  <si>
+    <t>Tue Sep 22 22:56:15 CEST 2020</t>
+  </si>
+  <si>
+    <t>Tue Sep 22 22:56:36 CEST 2020</t>
+  </si>
+  <si>
+    <t>Tue Sep 22 22:56:54 CEST 2020</t>
+  </si>
+  <si>
+    <t>Tue Sep 22 22:57:20 CEST 2020</t>
+  </si>
+  <si>
+    <t>Tue Sep 22 22:57:21 CEST 2020</t>
+  </si>
+  <si>
+    <t>Tue Sep 22 22:57:23 CEST 2020</t>
   </si>
 </sst>
 </file>
@@ -786,7 +822,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F125"/>
+  <dimension ref="A1:F132"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2919,6 +2955,146 @@
         <v>135</v>
       </c>
     </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>125.0</v>
+      </c>
+      <c r="B126" t="s">
+        <v>23</v>
+      </c>
+      <c r="C126" t="s">
+        <v>23</v>
+      </c>
+      <c r="D126" t="s">
+        <v>136</v>
+      </c>
+      <c r="E126" t="s">
+        <v>137</v>
+      </c>
+      <c r="F126" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>126.0</v>
+      </c>
+      <c r="B127" t="s">
+        <v>19</v>
+      </c>
+      <c r="C127" t="s">
+        <v>19</v>
+      </c>
+      <c r="D127" t="s">
+        <v>139</v>
+      </c>
+      <c r="E127" t="s">
+        <v>140</v>
+      </c>
+      <c r="F127" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>127.0</v>
+      </c>
+      <c r="B128" t="s">
+        <v>23</v>
+      </c>
+      <c r="C128" t="s">
+        <v>23</v>
+      </c>
+      <c r="D128" t="s">
+        <v>137</v>
+      </c>
+      <c r="E128" t="s">
+        <v>142</v>
+      </c>
+      <c r="F128" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>128.0</v>
+      </c>
+      <c r="B129" t="s">
+        <v>23</v>
+      </c>
+      <c r="C129" t="s">
+        <v>23</v>
+      </c>
+      <c r="D129" t="s">
+        <v>142</v>
+      </c>
+      <c r="E129" t="s">
+        <v>143</v>
+      </c>
+      <c r="F129" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>129.0</v>
+      </c>
+      <c r="B130" t="s">
+        <v>19</v>
+      </c>
+      <c r="C130" t="s">
+        <v>19</v>
+      </c>
+      <c r="D130" t="s">
+        <v>140</v>
+      </c>
+      <c r="E130" t="s">
+        <v>144</v>
+      </c>
+      <c r="F130" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>130.0</v>
+      </c>
+      <c r="B131" t="s">
+        <v>23</v>
+      </c>
+      <c r="C131" t="s">
+        <v>23</v>
+      </c>
+      <c r="D131" t="s">
+        <v>143</v>
+      </c>
+      <c r="E131" t="s">
+        <v>145</v>
+      </c>
+      <c r="F131" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>131.0</v>
+      </c>
+      <c r="B132" t="s">
+        <v>23</v>
+      </c>
+      <c r="C132" t="s">
+        <v>23</v>
+      </c>
+      <c r="D132" t="s">
+        <v>146</v>
+      </c>
+      <c r="E132" t="s">
+        <v>147</v>
+      </c>
+      <c r="F132" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>